<commit_message>
Tariff Added and Searchbox updated
</commit_message>
<xml_diff>
--- a/BillAppDocs/MonthlyUploadData.xlsx
+++ b/BillAppDocs/MonthlyUploadData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDir\Walee\Bill-Website-Walee\BillAppDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C292A4E-D9FF-4238-8DD1-259FEEE73C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11C80E0-B89F-4A20-A956-87A6AF6AFA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -354,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,6 +389,17 @@
         <v>15542</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>12345678901122</v>
+      </c>
+      <c r="B3">
+        <v>1860</v>
+      </c>
+      <c r="C3">
+        <v>9619</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Files upload sections updated
</commit_message>
<xml_diff>
--- a/BillAppDocs/MonthlyUploadData.xlsx
+++ b/BillAppDocs/MonthlyUploadData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDir\Walee\Bill-Website-Walee\BillAppDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11C80E0-B89F-4A20-A956-87A6AF6AFA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29B4E50-EAA2-4302-AC4E-BE99A07C8D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,13 +27,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>meterId</t>
-  </si>
-  <si>
     <t>present_peak_reading</t>
   </si>
   <si>
     <t>present_off_peak_reading</t>
+  </si>
+  <si>
+    <t>userId</t>
   </si>
 </sst>
 </file>
@@ -357,7 +357,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -369,18 +369,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>12345678901234</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>3916</v>
@@ -391,7 +391,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>12345678901122</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1860</v>

</xml_diff>

<commit_message>
tables update logic added
</commit_message>
<xml_diff>
--- a/BillAppDocs/MonthlyUploadData.xlsx
+++ b/BillAppDocs/MonthlyUploadData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDir\Walee\Bill-Website-Walee\BillAppDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29B4E50-EAA2-4302-AC4E-BE99A07C8D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44386E25-313A-40EE-939B-9A6F17BB4A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -357,7 +357,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
monthly upload data updated
</commit_message>
<xml_diff>
--- a/BillAppDocs/MonthlyUploadData.xlsx
+++ b/BillAppDocs/MonthlyUploadData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDir\Walee\Bill-Website-Walee\BillAppDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44386E25-313A-40EE-939B-9A6F17BB4A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE8B642-74B6-4B6E-8BD2-C75D36BA99DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>present_peak_reading</t>
   </si>
   <si>
-    <t>present_off_peak_reading</t>
+    <t>userId</t>
   </si>
   <si>
-    <t>userId</t>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>"Dec-24"</t>
+  </si>
+  <si>
+    <t>present_off_peak_reading</t>
   </si>
 </sst>
 </file>
@@ -69,11 +75,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -371,32 +378,40 @@
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>3916</v>
-      </c>
-      <c r="C2">
-        <v>15542</v>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3916</v>
+      </c>
+      <c r="C3">
+        <v>15542</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>1860</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>9619</v>
       </c>
     </row>

</xml_diff>

<commit_message>
file upload sections updated
</commit_message>
<xml_diff>
--- a/BillAppDocs/MonthlyUploadData.xlsx
+++ b/BillAppDocs/MonthlyUploadData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDir\Walee\Bill-Website-Walee\BillAppDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE8B642-74B6-4B6E-8BD2-C75D36BA99DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F451E8E5-337F-49B8-B4F6-B0ADE35DC450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -364,7 +364,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
admin login page upd
</commit_message>
<xml_diff>
--- a/BillAppDocs/MonthlyUploadData.xlsx
+++ b/BillAppDocs/MonthlyUploadData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDir\Walee\Bill-Website-Walee\BillAppDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4E28E8-0D94-4EB9-9622-6BA417761308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56EA397-1779-42D5-9FD0-4D9B60CDFE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -364,7 +364,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
toast added in all files
</commit_message>
<xml_diff>
--- a/BillAppDocs/MonthlyUploadData.xlsx
+++ b/BillAppDocs/MonthlyUploadData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDir\Walee\Bill-Website-Walee\BillAppDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56EA397-1779-42D5-9FD0-4D9B60CDFE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB22660-699D-4908-9E0F-4A0A14EC151D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -364,7 +364,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>